<commit_message>
feat: acao branch changes applyed
</commit_message>
<xml_diff>
--- a/data/Acao.xlsx
+++ b/data/Acao.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27109"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="404" documentId="11_BC30D1DE80CC4242E268565A893E8C1851039F94" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EF8AC47-4DAC-4BFF-BEDA-B2DD0E32FE0A}"/>
+  <xr:revisionPtr revIDLastSave="406" documentId="11_BC30D1DE80CC4242E268565A893E8C1851039F94" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45F87574-D17F-484F-9046-6722670AFE04}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
   <si>
     <t>VUhHovX86EGcSMJ9tFLW3eliBq_LQmRApCNJlTPGic1UQjhTOTQ5VllFUUNBMTdIUVVOOUNCMjRLTi4u</t>
   </si>
@@ -187,6 +187,36 @@
   </si>
   <si>
     <t>Extrajudicial;Relacionada a projeto institucional das unidades de apoio à atividade finalística;</t>
+  </si>
+  <si>
+    <t>apdan@mpes.mp.br</t>
+  </si>
+  <si>
+    <t>Ana Paula Senna Dan Rossoni</t>
+  </si>
+  <si>
+    <t>Criminal</t>
+  </si>
+  <si>
+    <t>Tráfico de drogas e crimes patrimoniais</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Consumidor</t>
+  </si>
+  <si>
+    <t>Proteção dos cidadãos nas relações de consumo</t>
+  </si>
+  <si>
+    <t>eejifhvdjka</t>
+  </si>
+  <si>
+    <t>teste</t>
+  </si>
+  <si>
+    <t>Extrajudicial;Judicial;Relacionada a projeto institucional das unidades de apoio à atividade finalística;</t>
   </si>
 </sst>
 </file>
@@ -226,13 +256,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -347,8 +380,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5DCC6897-D9C1-4C15-84F9-B6BA5FB5C920}" name="Tabela1" displayName="Tabela1" ref="A1:AD3" totalsRowShown="0" headerRowDxfId="30">
-  <autoFilter ref="A1:AD3" xr:uid="{5DCC6897-D9C1-4C15-84F9-B6BA5FB5C920}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5DCC6897-D9C1-4C15-84F9-B6BA5FB5C920}" name="Tabela1" displayName="Tabela1" ref="A1:AD5" totalsRowShown="0" headerRowDxfId="30">
+  <autoFilter ref="A1:AD5" xr:uid="{5DCC6897-D9C1-4C15-84F9-B6BA5FB5C920}"/>
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{6E9724C3-77DB-4F61-B2C5-898F962AD9D6}" name="ID" dataDxfId="29"/>
     <tableColumn id="2" xr3:uid="{3CFE0144-708E-4793-AE27-5E7E19E3B8AA}" name="Hora de início" dataDxfId="28"/>
@@ -712,7 +745,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89CB478E-B55E-4A8D-8DF0-99ABB7207F39}">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AD5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -815,7 +848,7 @@
       </c>
     </row>
     <row r="2" spans="1:30" ht="60.75">
-      <c r="A2" s="4">
+      <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2">
@@ -824,45 +857,29 @@
       <c r="C2" s="2">
         <v>45250.661516203705</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="4" t="s">
+      <c r="G2" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="5" t="s">
+      <c r="X2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Y2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="Z2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" t="s">
         <v>40</v>
       </c>
       <c r="AC2" s="3">
@@ -873,7 +890,7 @@
       </c>
     </row>
     <row r="3" spans="1:30">
-      <c r="A3" s="4">
+      <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2">
@@ -882,45 +899,29 @@
       <c r="C3" s="2">
         <v>45250.661851851852</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" t="s">
         <v>34</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="4" t="s">
+      <c r="G3" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4" t="s">
+      <c r="M3" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="5" t="s">
+      <c r="X3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="Y3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c r="Z3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4" t="s">
+      <c r="AB3" t="s">
         <v>46</v>
       </c>
       <c r="AC3" s="3">
@@ -928,6 +929,120 @@
       </c>
       <c r="AD3" s="3">
         <v>45254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45251.63013888889</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45251.630567129629</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="3">
+        <v>45260</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>45260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45251.630636574075</v>
+      </c>
+      <c r="C5" s="2">
+        <v>45251.630983796298</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>45259</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>45274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>